<commit_message>
start fix cart and cookie
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VB2\3. Ki.III\4. 77CG. Java 2\BTL\Mobileshop_SpringbootMVC_Thymeleaf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VB2\7. Git Code\Mobileshop_SpringbootMVC_Thymeleaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>1. Quản lý tài khoản (Đối với Admin)</t>
   </si>
@@ -38,9 +38,6 @@
     <t>2. Quản lý sản phẩm</t>
   </si>
   <si>
-    <t>2.1, Thêm điện thoại</t>
-  </si>
-  <si>
     <t>2.2. Sửa thông tin điện thoại</t>
   </si>
   <si>
@@ -111,6 +108,15 @@
   </si>
   <si>
     <t>3. Quản lý hàng tồn kho hoặc đã bán</t>
+  </si>
+  <si>
+    <t>2.1. Thêm điện thoại</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Chức năng</t>
   </si>
 </sst>
 </file>
@@ -438,160 +444,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
+      <c r="A19" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
+      <c r="A21" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>26</v>
+      <c r="A28" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>